<commit_message>
Realestate Update resale numbers to the xslx file 2023-05-27 23:43
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -1,127 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitee\pyradnotes\source\Notes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="11880"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="21585" windowHeight="11880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="CityResaleNum" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CityResaleNum" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Weekday</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Beijing</t>
-  </si>
-  <si>
-    <t>Guangzhou</t>
-  </si>
-  <si>
-    <t>Suzhou</t>
-  </si>
-  <si>
-    <t>Hangzhou</t>
-  </si>
-  <si>
-    <t>Nanjing</t>
-  </si>
-  <si>
-    <t>Xi_an</t>
-  </si>
-  <si>
-    <t>Chengdu</t>
-  </si>
-  <si>
-    <t>Chongqing</t>
-  </si>
-  <si>
-    <t>Tianjin</t>
-  </si>
-  <si>
-    <t>Hefei</t>
-  </si>
-  <si>
-    <t>Fuzhou</t>
-  </si>
-  <si>
-    <t>Xiamen</t>
-  </si>
-  <si>
-    <t>Changsha</t>
-  </si>
-  <si>
-    <t>Shanghai</t>
-  </si>
-  <si>
-    <t>Shenzhen</t>
-  </si>
-  <si>
-    <t>Wuhan</t>
-  </si>
-  <si>
-    <t>2023-05-26</t>
-  </si>
-  <si>
-    <t>23:15:12</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -155,24 +74,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -460,157 +438,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
-    <col min="5" max="5" width="9.75" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="9.25" customWidth="1"/>
-    <col min="12" max="12" width="11.125" customWidth="1"/>
-    <col min="17" max="17" width="11.25" customWidth="1"/>
-    <col min="18" max="18" width="12.625" customWidth="1"/>
-    <col min="19" max="19" width="11.75" customWidth="1"/>
+    <col width="13.625" customWidth="1" min="1" max="1"/>
+    <col width="12.125" customWidth="1" min="2" max="2"/>
+    <col width="13.375" customWidth="1" min="3" max="3"/>
+    <col width="11.25" customWidth="1" min="4" max="4"/>
+    <col width="9.75" customWidth="1" min="5" max="5"/>
+    <col width="12.125" customWidth="1" min="6" max="6"/>
+    <col width="9.5" customWidth="1" min="7" max="7"/>
+    <col width="10.5" customWidth="1" min="8" max="8"/>
+    <col width="9.25" customWidth="1" min="11" max="11"/>
+    <col width="11.125" customWidth="1" min="12" max="12"/>
+    <col width="11.25" customWidth="1" min="17" max="17"/>
+    <col width="12.625" customWidth="1" min="18" max="18"/>
+    <col width="11.75" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Week</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Beijing</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Guangzhou</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Suzhou</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Hangzhou</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Nanjing</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Xi_an</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Chengdu</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Chongqing</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Tianjin</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Hefei</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Fuzhou</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Xiamen</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Changsha</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Shanghai</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Shenzhen</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Wuhan</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-05-26</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>23:15:12</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>119669</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>133088</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>157247</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>131037</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>174019</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="n">
         <v>113784</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="n">
         <v>197840</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="n">
         <v>219269</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="n">
         <v>171594</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="n">
         <v>119342</v>
       </c>
-      <c r="O2">
+      <c r="O2" t="n">
         <v>38554</v>
       </c>
-      <c r="P2">
+      <c r="P2" t="n">
         <v>34858</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" t="n">
         <v>50285</v>
       </c>
-      <c r="R2">
+      <c r="R2" t="n">
         <v>-1</v>
       </c>
-      <c r="S2">
+      <c r="S2" t="n">
         <v>36931</v>
       </c>
-      <c r="T2">
+      <c r="T2" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-05-27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>23:41:53</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>119793</v>
+      </c>
+      <c r="F3" t="n">
+        <v>133223</v>
+      </c>
+      <c r="G3" t="n">
+        <v>157601</v>
+      </c>
+      <c r="H3" t="n">
+        <v>130967</v>
+      </c>
+      <c r="I3" t="n">
+        <v>174166</v>
+      </c>
+      <c r="J3" t="n">
+        <v>114091</v>
+      </c>
+      <c r="K3" t="n">
+        <v>198073</v>
+      </c>
+      <c r="L3" t="n">
+        <v>219730</v>
+      </c>
+      <c r="M3" t="n">
+        <v>171920</v>
+      </c>
+      <c r="N3" t="n">
+        <v>119577</v>
+      </c>
+      <c r="O3" t="n">
+        <v>38556</v>
+      </c>
+      <c r="P3" t="n">
+        <v>34908</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>50368</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>37009</v>
+      </c>
+      <c r="T3" t="n">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Realestate Update resale numbers to the xlsx file 2023-05-28 15:09
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -708,6 +708,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-05-28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>15:06:41</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>119926</v>
+      </c>
+      <c r="F4" t="n">
+        <v>133334</v>
+      </c>
+      <c r="G4" t="n">
+        <v>157695</v>
+      </c>
+      <c r="H4" t="n">
+        <v>130849</v>
+      </c>
+      <c r="I4" t="n">
+        <v>174265</v>
+      </c>
+      <c r="J4" t="n">
+        <v>114242</v>
+      </c>
+      <c r="K4" t="n">
+        <v>198116</v>
+      </c>
+      <c r="L4" t="n">
+        <v>219609</v>
+      </c>
+      <c r="M4" t="n">
+        <v>171953</v>
+      </c>
+      <c r="N4" t="n">
+        <v>119654</v>
+      </c>
+      <c r="O4" t="n">
+        <v>38541</v>
+      </c>
+      <c r="P4" t="n">
+        <v>34916</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>50339</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>36871</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers to xlsx & md files 2023-05-28 22:12
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -778,6 +778,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-05-28</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22:07:21</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>119957</v>
+      </c>
+      <c r="F5" t="n">
+        <v>133322</v>
+      </c>
+      <c r="G5" t="n">
+        <v>157974</v>
+      </c>
+      <c r="H5" t="n">
+        <v>130719</v>
+      </c>
+      <c r="I5" t="n">
+        <v>174322</v>
+      </c>
+      <c r="J5" t="n">
+        <v>114355</v>
+      </c>
+      <c r="K5" t="n">
+        <v>198289</v>
+      </c>
+      <c r="L5" t="n">
+        <v>219973</v>
+      </c>
+      <c r="M5" t="n">
+        <v>172034</v>
+      </c>
+      <c r="N5" t="n">
+        <v>119759</v>
+      </c>
+      <c r="O5" t="n">
+        <v>38627</v>
+      </c>
+      <c r="P5" t="n">
+        <v>34955</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>50395</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>37182</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers to the xlsx file 2023-05-29 10:27
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -848,6 +848,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:24:58</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>119562</v>
+      </c>
+      <c r="F6" t="n">
+        <v>133603</v>
+      </c>
+      <c r="G6" t="n">
+        <v>157812</v>
+      </c>
+      <c r="H6" t="n">
+        <v>130683</v>
+      </c>
+      <c r="I6" t="n">
+        <v>174324</v>
+      </c>
+      <c r="J6" t="n">
+        <v>113280</v>
+      </c>
+      <c r="K6" t="n">
+        <v>198205</v>
+      </c>
+      <c r="L6" t="n">
+        <v>219955</v>
+      </c>
+      <c r="M6" t="n">
+        <v>172219</v>
+      </c>
+      <c r="N6" t="n">
+        <v>119843</v>
+      </c>
+      <c r="O6" t="n">
+        <v>38587</v>
+      </c>
+      <c r="P6" t="n">
+        <v>34923</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>50370</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>36790</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-05-29 22:41
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -918,6 +918,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-05-29</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>22:37:42</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>119787</v>
+      </c>
+      <c r="F7" t="n">
+        <v>133521</v>
+      </c>
+      <c r="G7" t="n">
+        <v>158308</v>
+      </c>
+      <c r="H7" t="n">
+        <v>130536</v>
+      </c>
+      <c r="I7" t="n">
+        <v>174464</v>
+      </c>
+      <c r="J7" t="n">
+        <v>113825</v>
+      </c>
+      <c r="K7" t="n">
+        <v>198314</v>
+      </c>
+      <c r="L7" t="n">
+        <v>220243</v>
+      </c>
+      <c r="M7" t="n">
+        <v>172080</v>
+      </c>
+      <c r="N7" t="n">
+        <v>119833</v>
+      </c>
+      <c r="O7" t="n">
+        <v>38681</v>
+      </c>
+      <c r="P7" t="n">
+        <v>34857</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>50423</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>36969</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-05-30 14:07
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -988,6 +988,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-05-30</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>14:05:52</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>119835</v>
+      </c>
+      <c r="F8" t="n">
+        <v>133541</v>
+      </c>
+      <c r="G8" t="n">
+        <v>158282</v>
+      </c>
+      <c r="H8" t="n">
+        <v>130822</v>
+      </c>
+      <c r="I8" t="n">
+        <v>174497</v>
+      </c>
+      <c r="J8" t="n">
+        <v>113620</v>
+      </c>
+      <c r="K8" t="n">
+        <v>198303</v>
+      </c>
+      <c r="L8" t="n">
+        <v>220206</v>
+      </c>
+      <c r="M8" t="n">
+        <v>171994</v>
+      </c>
+      <c r="N8" t="n">
+        <v>119875</v>
+      </c>
+      <c r="O8" t="n">
+        <v>38604</v>
+      </c>
+      <c r="P8" t="n">
+        <v>34861</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>50503</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>36734</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-05-30 22:10
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1058,6 +1058,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-05-30</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>22:07:01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>119934</v>
+      </c>
+      <c r="F9" t="n">
+        <v>133553</v>
+      </c>
+      <c r="G9" t="n">
+        <v>158433</v>
+      </c>
+      <c r="H9" t="n">
+        <v>130842</v>
+      </c>
+      <c r="I9" t="n">
+        <v>174624</v>
+      </c>
+      <c r="J9" t="n">
+        <v>113750</v>
+      </c>
+      <c r="K9" t="n">
+        <v>198644</v>
+      </c>
+      <c r="L9" t="n">
+        <v>220588</v>
+      </c>
+      <c r="M9" t="n">
+        <v>171963</v>
+      </c>
+      <c r="N9" t="n">
+        <v>119871</v>
+      </c>
+      <c r="O9" t="n">
+        <v>38707</v>
+      </c>
+      <c r="P9" t="n">
+        <v>34826</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>50540</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>36931</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-05-31 19:36
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1268,6 +1268,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-05-31</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>19:35:13</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>120245</v>
+      </c>
+      <c r="F12" t="n">
+        <v>133429</v>
+      </c>
+      <c r="G12" t="n">
+        <v>158933</v>
+      </c>
+      <c r="H12" t="n">
+        <v>131036</v>
+      </c>
+      <c r="I12" t="n">
+        <v>174858</v>
+      </c>
+      <c r="J12" t="n">
+        <v>113868</v>
+      </c>
+      <c r="K12" t="n">
+        <v>198821</v>
+      </c>
+      <c r="L12" t="n">
+        <v>220315</v>
+      </c>
+      <c r="M12" t="n">
+        <v>172024</v>
+      </c>
+      <c r="N12" t="n">
+        <v>120097</v>
+      </c>
+      <c r="O12" t="n">
+        <v>38710</v>
+      </c>
+      <c r="P12" t="n">
+        <v>34887</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>50637</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S12" t="n">
+        <v>36878</v>
+      </c>
+      <c r="T12" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-05-31 21:38
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1338,6 +1338,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-05-31</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>21:36:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>120271</v>
+      </c>
+      <c r="F13" t="n">
+        <v>133519</v>
+      </c>
+      <c r="G13" t="n">
+        <v>158974</v>
+      </c>
+      <c r="H13" t="n">
+        <v>130957</v>
+      </c>
+      <c r="I13" t="n">
+        <v>174859</v>
+      </c>
+      <c r="J13" t="n">
+        <v>113878</v>
+      </c>
+      <c r="K13" t="n">
+        <v>198929</v>
+      </c>
+      <c r="L13" t="n">
+        <v>220338</v>
+      </c>
+      <c r="M13" t="n">
+        <v>172243</v>
+      </c>
+      <c r="N13" t="n">
+        <v>120038</v>
+      </c>
+      <c r="O13" t="n">
+        <v>38729</v>
+      </c>
+      <c r="P13" t="n">
+        <v>34925</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>50654</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S13" t="n">
+        <v>36961</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-06-01 19:45
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1408,6 +1408,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>19:43:03</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>120516</v>
+      </c>
+      <c r="F14" t="n">
+        <v>133763</v>
+      </c>
+      <c r="G14" t="n">
+        <v>158220</v>
+      </c>
+      <c r="H14" t="n">
+        <v>129338</v>
+      </c>
+      <c r="I14" t="n">
+        <v>173929</v>
+      </c>
+      <c r="J14" t="n">
+        <v>111686</v>
+      </c>
+      <c r="K14" t="n">
+        <v>198924</v>
+      </c>
+      <c r="L14" t="n">
+        <v>217494</v>
+      </c>
+      <c r="M14" t="n">
+        <v>170584</v>
+      </c>
+      <c r="N14" t="n">
+        <v>118211</v>
+      </c>
+      <c r="O14" t="n">
+        <v>37859</v>
+      </c>
+      <c r="P14" t="n">
+        <v>34930</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>49946</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S14" t="n">
+        <v>36733</v>
+      </c>
+      <c r="T14" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-06-02 16:33
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1478,6 +1478,146 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-06-02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10:16:34</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>120492</v>
+      </c>
+      <c r="F15" t="n">
+        <v>133982</v>
+      </c>
+      <c r="G15" t="n">
+        <v>158003</v>
+      </c>
+      <c r="H15" t="n">
+        <v>129556</v>
+      </c>
+      <c r="I15" t="n">
+        <v>174025</v>
+      </c>
+      <c r="J15" t="n">
+        <v>111624</v>
+      </c>
+      <c r="K15" t="n">
+        <v>198997</v>
+      </c>
+      <c r="L15" t="n">
+        <v>217488</v>
+      </c>
+      <c r="M15" t="n">
+        <v>170999</v>
+      </c>
+      <c r="N15" t="n">
+        <v>118375</v>
+      </c>
+      <c r="O15" t="n">
+        <v>37878</v>
+      </c>
+      <c r="P15" t="n">
+        <v>34893</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>49993</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>36370</v>
+      </c>
+      <c r="T15" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-06-02</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:32:08</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>120621</v>
+      </c>
+      <c r="F16" t="n">
+        <v>133845</v>
+      </c>
+      <c r="G16" t="n">
+        <v>158538</v>
+      </c>
+      <c r="H16" t="n">
+        <v>130038</v>
+      </c>
+      <c r="I16" t="n">
+        <v>174274</v>
+      </c>
+      <c r="J16" t="n">
+        <v>112011</v>
+      </c>
+      <c r="K16" t="n">
+        <v>199359</v>
+      </c>
+      <c r="L16" t="n">
+        <v>217948</v>
+      </c>
+      <c r="M16" t="n">
+        <v>171156</v>
+      </c>
+      <c r="N16" t="n">
+        <v>118531</v>
+      </c>
+      <c r="O16" t="n">
+        <v>37968</v>
+      </c>
+      <c r="P16" t="n">
+        <v>34867</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>50103</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>36674</v>
+      </c>
+      <c r="T16" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-06-02 22:24
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1618,6 +1618,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-06-02</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>22:21:34</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>120654</v>
+      </c>
+      <c r="F17" t="n">
+        <v>133793</v>
+      </c>
+      <c r="G17" t="n">
+        <v>158797</v>
+      </c>
+      <c r="H17" t="n">
+        <v>130163</v>
+      </c>
+      <c r="I17" t="n">
+        <v>174389</v>
+      </c>
+      <c r="J17" t="n">
+        <v>112238</v>
+      </c>
+      <c r="K17" t="n">
+        <v>199466</v>
+      </c>
+      <c r="L17" t="n">
+        <v>218299</v>
+      </c>
+      <c r="M17" t="n">
+        <v>171424</v>
+      </c>
+      <c r="N17" t="n">
+        <v>118670</v>
+      </c>
+      <c r="O17" t="n">
+        <v>38052</v>
+      </c>
+      <c r="P17" t="n">
+        <v>34846</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>50068</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>36899</v>
+      </c>
+      <c r="T17" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>

<commit_message>
Realestate Update resale numbers 2023-06-03 13:48
</commit_message>
<xml_diff>
--- a/source/Notes/cityResaleNum16.xlsx
+++ b/source/Notes/cityResaleNum16.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1688,6 +1688,76 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-06-03</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>13:47:07</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>120763</v>
+      </c>
+      <c r="F18" t="n">
+        <v>133945</v>
+      </c>
+      <c r="G18" t="n">
+        <v>158821</v>
+      </c>
+      <c r="H18" t="n">
+        <v>130334</v>
+      </c>
+      <c r="I18" t="n">
+        <v>174588</v>
+      </c>
+      <c r="J18" t="n">
+        <v>112471</v>
+      </c>
+      <c r="K18" t="n">
+        <v>199541</v>
+      </c>
+      <c r="L18" t="n">
+        <v>218447</v>
+      </c>
+      <c r="M18" t="n">
+        <v>171690</v>
+      </c>
+      <c r="N18" t="n">
+        <v>118828</v>
+      </c>
+      <c r="O18" t="n">
+        <v>38082</v>
+      </c>
+      <c r="P18" t="n">
+        <v>34825</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>50146</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>36712</v>
+      </c>
+      <c r="T18" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>